<commit_message>
added a new exclusion template
</commit_message>
<xml_diff>
--- a/Projects/JNJANZ/Data/KPI Exclusions Template.xlsx
+++ b/Projects/JNJANZ/Data/KPI Exclusions Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">product_name</t>
   </si>
   <si>
-    <t xml:space="preserve">Empty; Irrelevant</t>
+    <t xml:space="preserve">Empty; Irrelevant; General Empty</t>
   </si>
   <si>
     <t xml:space="preserve">eye_hand_level_sos</t>
@@ -304,14 +304,14 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.5627530364373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8825910931174"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
PROS-13942-JnJANZ - Exclude Sub Category-Update Config Template
</commit_message>
<xml_diff>
--- a/Projects/JNJANZ/Data/KPI Exclusions Template.xlsx
+++ b/Projects/JNJANZ/Data/KPI Exclusions Template.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t xml:space="preserve">Empty; Irrelevant; General Empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Out of Scope</t>
   </si>
   <si>
     <t xml:space="preserve">eye_hand_level_sos</t>
@@ -304,14 +310,14 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.2024291497976"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -342,10 +348,16 @@
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
@@ -356,12 +368,12 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PROS-14794] Template update for KPI-linear_product_length_out_of_store to exclude sub_category:Out of Scope
</commit_message>
<xml_diff>
--- a/Projects/JNJANZ/Data/KPI Exclusions Template.xlsx
+++ b/Projects/JNJANZ/Data/KPI Exclusions Template.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">promo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linear_product_length_out_of_store</t>
   </si>
 </sst>
 </file>
@@ -307,18 +310,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.2024291497976"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.4655870445344"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.0607287449393"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4898785425101"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -374,6 +378,23 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PROS-14942] Sand-to-Prod Preparing for prod deployment
</commit_message>
<xml_diff>
--- a/Projects/JNJANZ/Data/KPI Exclusions Template.xlsx
+++ b/Projects/JNJANZ/Data/KPI Exclusions Template.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">linear_product_length_out_of_store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribution</t>
   </si>
 </sst>
 </file>
@@ -310,18 +313,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.4655870445344"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.0607287449393"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4898785425101"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.4898785425101"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -395,6 +398,11 @@
       </c>
       <c r="E6" s="0" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>